<commit_message>
1) Updated the PPS330D BOM to reflect package and ordering changes 2) Updated the PRIME BOM to include the LCD under consideration
</commit_message>
<xml_diff>
--- a/Hardware/LAB-PPS330D/docs/LAB-PPS330DR0-Rev1BOM.xlsx
+++ b/Hardware/LAB-PPS330D/docs/LAB-PPS330DR0-Rev1BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6336" yWindow="-24" windowWidth="18348" windowHeight="13440" activeTab="1"/>
+    <workbookView xWindow="8580" yWindow="-24" windowWidth="18348" windowHeight="13440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -351,12 +350,6 @@
     <t>8-DSBGA</t>
   </si>
   <si>
-    <t>296-21059-1-ND</t>
-  </si>
-  <si>
-    <t>SN74LVC1G139YZPR</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -375,12 +368,6 @@
     <t>MOSFET N/P-CH 20V 3A/2.2A SSOT-6</t>
   </si>
   <si>
-    <t>FDC6420CDKR-ND</t>
-  </si>
-  <si>
-    <t>FDC6312PDKR-ND</t>
-  </si>
-  <si>
     <t>MOSFET 2P-CH 20V 2.3A SSOT-6</t>
   </si>
   <si>
@@ -391,6 +378,18 @@
   </si>
   <si>
     <t>U4</t>
+  </si>
+  <si>
+    <t>296-18203-1-ND</t>
+  </si>
+  <si>
+    <t>FDC6312PCT-ND</t>
+  </si>
+  <si>
+    <t>FDC6420CCT-ND</t>
+  </si>
+  <si>
+    <t>SN74LVC1G139DCU</t>
   </si>
 </sst>
 </file>
@@ -1460,7 +1459,7 @@
         <v>83</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D6" s="31"/>
       <c r="E6" s="3"/>
@@ -1515,7 +1514,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>98</v>
@@ -1564,7 +1563,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>92</v>
@@ -1585,7 +1584,7 @@
         <v>104</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -1593,19 +1592,19 @@
         <v>4</v>
       </c>
       <c r="B12" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="D12" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="D12" s="22" t="s">
-        <v>119</v>
-      </c>
       <c r="E12" s="22" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G12" s="21">
         <v>2</v>
@@ -1615,7 +1614,7 @@
         <v>104</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1623,19 +1622,19 @@
         <v>5</v>
       </c>
       <c r="B13" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="C13" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="D13" s="22" t="s">
+      <c r="E13" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="E13" s="22" t="s">
-        <v>120</v>
-      </c>
       <c r="F13" s="23" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G13" s="21">
         <v>1</v>
@@ -1645,7 +1644,7 @@
         <v>104</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1921,11 +1920,11 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J10" r:id="rId1" display="http://www.digikey.com/product-detail/en/PRPC040SAAN-RC/S1011EC-40-ND/2775214"/>
-    <hyperlink ref="J11" r:id="rId2" display="http://www.digikey.com/product-detail/en/SN74LVC1G139YZPR/296-21059-1-ND/1217016"/>
-    <hyperlink ref="B12" r:id="rId3" display="http://www.digikey.com/product-detail/en/FDC6312P/FDC6312PTR-ND/979786"/>
-    <hyperlink ref="B13" r:id="rId4" display="http://www.digikey.com/product-detail/en/FDC6420C/FDC6420CDKR-ND/1849945"/>
-    <hyperlink ref="J13" r:id="rId5" display="http://www.digikey.com/product-detail/en/FDC6420C/FDC6420CDKR-ND/1849945"/>
-    <hyperlink ref="J12" r:id="rId6" display="http://www.digikey.com/product-detail/en/FDC6312P/FDC6312PDKR-ND/1626343"/>
+    <hyperlink ref="B12" r:id="rId2" display="http://www.digikey.com/product-detail/en/FDC6312P/FDC6312PTR-ND/979786"/>
+    <hyperlink ref="B13" r:id="rId3" display="http://www.digikey.com/product-detail/en/FDC6420C/FDC6420CDKR-ND/1849945"/>
+    <hyperlink ref="J11" r:id="rId4" display="http://www.digikey.com/product-detail/en/SN74LVC1G139DCUR/296-18203-1-ND/772127"/>
+    <hyperlink ref="J12" r:id="rId5" display="http://www.digikey.com/product-detail/en/FDC6312P/FDC6312PCT-ND/1626187"/>
+    <hyperlink ref="J13" r:id="rId6" display="http://www.digikey.com/product-detail/en/FDC6420C/FDC6420CCT-ND/1849901"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="50" orientation="landscape" r:id="rId7"/>

</xml_diff>